<commit_message>
Xong phan Ho so benh an
</commit_message>
<xml_diff>
--- a/Quá Trình/Kế hoạch.xlsx
+++ b/Quá Trình/Kế hoạch.xlsx
@@ -1386,10 +1386,10 @@
   <dimension ref="A1:Y43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomRight" activeCell="C21" sqref="C21:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2711,8 +2711,8 @@
       <c r="J19" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="K19">
-        <v>0</v>
+      <c r="K19" s="4">
+        <v>100</v>
       </c>
       <c r="L19">
         <v>3</v>

</xml_diff>